<commit_message>
I fixed the template so the exclusion will work as design.
</commit_message>
<xml_diff>
--- a/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Category </t>
+    <t xml:space="preserve">sub_category</t>
   </si>
   <si>
     <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
@@ -301,17 +301,17 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0971659919028"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="206.769230769231"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2591093117409"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="208.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update exclusion template for jnjuk
</commit_message>
<xml_diff>
--- a/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">linear_product_length_out_of_store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; KIDS COUGH ;  KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ;  KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBITOTICS ; PAIN MANAGEMENT ; FIRST AID ; MIGRAINE RELIEF ; RASH TREATMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ; BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ; KIDS WIPES ; BABY SUNCARE ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH</t>
   </si>
 </sst>
 </file>
@@ -89,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -119,6 +125,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -196,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,6 +237,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -298,19 +324,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="208.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8421052631579"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="210.595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -340,6 +366,17 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replace exclusion template in jnjuk and fix sanity test
</commit_message>
<xml_diff>
--- a/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUK/Data/KPI Exclusions Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -79,13 +79,7 @@
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
-    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">linear_product_length_out_of_store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; KIDS COUGH ;  KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ;  KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBITOTICS ; PAIN MANAGEMENT ; FIRST AID ; MIGRAINE RELIEF ; RASH TREATMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ; BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ; KIDS WIPES ; BABY SUNCARE ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH</t>
+    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; KIDS COUGH ;  KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ;  KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ;  REHYDRATION ; PROBITOTICS ; PAIN MANAGEMENT ; FIRST AID ; MIGRAINE RELIEF ; RASH TREATMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ; BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ; KIDS WIPES ; BABY SUNCARE ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH</t>
   </si>
 </sst>
 </file>
@@ -95,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,12 +124,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -214,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,16 +223,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -324,19 +304,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="210.595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="212.522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -357,7 +337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -368,17 +348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>